<commit_message>
improvements parser and tests
</commit_message>
<xml_diff>
--- a/inflation-resources/data/test_links_small_migros.xlsx
+++ b/inflation-resources/data/test_links_small_migros.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">item_code</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">product_links</t>
   </si>
   <si>
+    <t xml:space="preserve">0111101</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pirinç</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t xml:space="preserve">https://www.migros.com.tr/yayla-baldo-pirinc-1-kg-gonen-bolgesi-mahsulu-p-f7441</t>
   </si>
   <si>
+    <t xml:space="preserve">0111201</t>
+  </si>
+  <si>
     <t xml:space="preserve">Buğday Unu</t>
   </si>
   <si>
@@ -52,6 +58,9 @@
     <t xml:space="preserve">https://www.migros.com.tr/soke-tam-bugday-unu-1-kg-p-4c73f6</t>
   </si>
   <si>
+    <t xml:space="preserve">0111208</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bebek Maması (Toz Karışım)</t>
   </si>
   <si>
@@ -59,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.migros.com.tr/bebelac-devam-sutu-1-400-g-p-4cec83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0111209</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgur</t>
@@ -201,10 +213,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.37"/>
@@ -226,59 +238,59 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>111101</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>111201</v>
+      <c r="A3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>111208</v>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>111209</v>
+      <c r="A5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>